<commit_message>
Change the first version
</commit_message>
<xml_diff>
--- a/dummyExcel.xlsx
+++ b/dummyExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ynzhy/Desktop/gitExcel/testExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF5A99AA-36BF-3A49-87B7-E97B0EF8AF47}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F1992FC1-B7C3-E149-9CA8-A184B5FE2ED9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20380" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{1297C5F9-1265-D54A-8300-4000D6F7288E}"/>
   </bookViews>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27AA4D9F-ABE7-5C4A-B271-8118E6497A90}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -387,6 +387,14 @@
         <v>456</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>321</v>
+      </c>
+      <c r="B2">
+        <v>654</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add formula to spreadsheet
</commit_message>
<xml_diff>
--- a/dummyExcel.xlsx
+++ b/dummyExcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ynzhy/Desktop/gitExcel/testExcel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ynzhy/Desktop/gitExcel2/testExcel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F1992FC1-B7C3-E149-9CA8-A184B5FE2ED9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A32D7644-BCA4-304E-A8B3-5FCC2C4A4B66}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{1297C5F9-1265-D54A-8300-4000D6F7288E}"/>
+    <workbookView xWindow="40060" yWindow="5740" windowWidth="28040" windowHeight="17440" xr2:uid="{1297C5F9-1265-D54A-8300-4000D6F7288E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -392,7 +392,8 @@
         <v>321</v>
       </c>
       <c r="B2">
-        <v>654</v>
+        <f>B1*2</f>
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>